<commit_message>
amended related work section
</commit_message>
<xml_diff>
--- a/ThesisMasterDocument/research/conferencesAndEntities.xlsx
+++ b/ThesisMasterDocument/research/conferencesAndEntities.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\__THESIS\ThesisMasterDocument\research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E20463FE-708F-4B2F-8C4F-038184C5691A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8B9AE86-FA99-4694-B105-2D0CF0D3B323}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1035" yWindow="300" windowWidth="29745" windowHeight="19035" xr2:uid="{43808FCA-5A1B-46A4-BA1C-87A55419837E}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>https://conferenceindex.org/conferences/brain-computer-interfaces</t>
   </si>
@@ -154,6 +154,12 @@
   </si>
   <si>
     <t>Human Machine Interface</t>
+  </si>
+  <si>
+    <t>NeurIPS</t>
+  </si>
+  <si>
+    <t>https://neurips.cc/</t>
   </si>
 </sst>
 </file>
@@ -517,7 +523,7 @@
   <dimension ref="B2:T37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T11" sqref="T11"/>
+      <selection activeCell="T21" sqref="T21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -643,26 +649,36 @@
         <v>35</v>
       </c>
     </row>
+    <row r="21" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="S21" t="s">
+        <v>40</v>
+      </c>
+      <c r="T21" t="s">
+        <v>41</v>
+      </c>
+    </row>
     <row r="22" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>23</v>
       </c>
-      <c r="S22" s="1" t="s">
+    </row>
+    <row r="23" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="S23" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="23" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="S23" t="s">
+    <row r="24" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="S24" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="25" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="S25" s="1" t="s">
+    <row r="26" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="S26" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="26" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="S26" t="s">
+    <row r="27" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="S27" t="s">
         <v>33</v>
       </c>
     </row>
@@ -671,22 +687,20 @@
         <v>36</v>
       </c>
     </row>
-    <row r="34" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="S34" t="s">
-        <v>29</v>
-      </c>
-    </row>
     <row r="35" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="s">
         <v>37</v>
       </c>
       <c r="S35" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="36" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>38</v>
+      </c>
+      <c r="S36" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="37" spans="2:19" x14ac:dyDescent="0.25">

</xml_diff>